<commit_message>
Reordering, added gen_long_term and discussion_example.
</commit_message>
<xml_diff>
--- a/p_arrs/p_arr_1_row_40_20_col_2_lp_1_chisq.xlsx
+++ b/p_arrs/p_arr_1_row_40_20_col_2_lp_1_chisq.xlsx
@@ -2977,7 +2977,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="7">
@@ -2985,7 +2985,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="8">
@@ -2993,7 +2993,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="9">
@@ -3001,7 +3001,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="10">
@@ -3009,7 +3009,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="11">
@@ -3017,7 +3017,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="12">
@@ -3113,7 +3113,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -3121,7 +3121,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -3129,7 +3129,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -3137,7 +3137,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -3145,7 +3145,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -3273,7 +3273,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="44">
@@ -3337,7 +3337,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="52">
@@ -3345,7 +3345,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="53">
@@ -3353,7 +3353,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="54">
@@ -3361,7 +3361,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="55">
@@ -3369,7 +3369,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="56">
@@ -3377,7 +3377,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="57">
@@ -3385,7 +3385,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="58">
@@ -3449,7 +3449,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -3457,7 +3457,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -3465,7 +3465,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -3473,7 +3473,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -3481,7 +3481,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -3489,7 +3489,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -3497,7 +3497,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -3601,7 +3601,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="85">
@@ -3609,7 +3609,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="86">
@@ -3681,7 +3681,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="95">
@@ -3689,7 +3689,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="96">
@@ -3697,7 +3697,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="97">
@@ -3705,7 +3705,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="98">
@@ -3713,7 +3713,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="99">
@@ -3721,7 +3721,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="100">
@@ -3729,7 +3729,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="101">
@@ -3785,7 +3785,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -3793,7 +3793,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -3801,7 +3801,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -3809,7 +3809,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -3817,7 +3817,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -3825,7 +3825,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -3833,7 +3833,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -3841,7 +3841,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -3849,7 +3849,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -3929,7 +3929,7 @@
         <v>125</v>
       </c>
       <c r="B125" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="126">
@@ -3937,7 +3937,7 @@
         <v>126</v>
       </c>
       <c r="B126" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="127">
@@ -3945,7 +3945,7 @@
         <v>127</v>
       </c>
       <c r="B127" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="128">
@@ -4033,7 +4033,7 @@
         <v>138</v>
       </c>
       <c r="B138" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="139">
@@ -4041,7 +4041,7 @@
         <v>139</v>
       </c>
       <c r="B139" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="140">
@@ -4049,7 +4049,7 @@
         <v>140</v>
       </c>
       <c r="B140" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="141">
@@ -4057,7 +4057,7 @@
         <v>141</v>
       </c>
       <c r="B141" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="142">
@@ -4065,7 +4065,7 @@
         <v>142</v>
       </c>
       <c r="B142" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="143">
@@ -4073,7 +4073,7 @@
         <v>143</v>
       </c>
       <c r="B143" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="144">
@@ -4081,7 +4081,7 @@
         <v>144</v>
       </c>
       <c r="B144" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="145">
@@ -4121,7 +4121,7 @@
         <v>149</v>
       </c>
       <c r="B149" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -4129,7 +4129,7 @@
         <v>150</v>
       </c>
       <c r="B150" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -4137,7 +4137,7 @@
         <v>151</v>
       </c>
       <c r="B151" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -4145,7 +4145,7 @@
         <v>152</v>
       </c>
       <c r="B152" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -4153,7 +4153,7 @@
         <v>153</v>
       </c>
       <c r="B153" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -4161,7 +4161,7 @@
         <v>154</v>
       </c>
       <c r="B154" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -4169,7 +4169,7 @@
         <v>155</v>
       </c>
       <c r="B155" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -4177,7 +4177,7 @@
         <v>156</v>
       </c>
       <c r="B156" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -4185,7 +4185,7 @@
         <v>157</v>
       </c>
       <c r="B157" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -4193,7 +4193,7 @@
         <v>158</v>
       </c>
       <c r="B158" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -4265,7 +4265,7 @@
         <v>167</v>
       </c>
       <c r="B167" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="168">
@@ -4273,7 +4273,7 @@
         <v>168</v>
       </c>
       <c r="B168" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="169">
@@ -4281,7 +4281,7 @@
         <v>169</v>
       </c>
       <c r="B169" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="170">
@@ -4377,7 +4377,7 @@
         <v>181</v>
       </c>
       <c r="B181" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="182">
@@ -4385,7 +4385,7 @@
         <v>182</v>
       </c>
       <c r="B182" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="183">
@@ -4393,7 +4393,7 @@
         <v>183</v>
       </c>
       <c r="B183" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="184">
@@ -4401,7 +4401,7 @@
         <v>184</v>
       </c>
       <c r="B184" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="185">
@@ -4409,7 +4409,7 @@
         <v>185</v>
       </c>
       <c r="B185" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="186">
@@ -4417,7 +4417,7 @@
         <v>186</v>
       </c>
       <c r="B186" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="187">
@@ -4425,7 +4425,7 @@
         <v>187</v>
       </c>
       <c r="B187" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="188">
@@ -4457,7 +4457,7 @@
         <v>191</v>
       </c>
       <c r="B191" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -4465,7 +4465,7 @@
         <v>192</v>
       </c>
       <c r="B192" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -4473,7 +4473,7 @@
         <v>193</v>
       </c>
       <c r="B193" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194">
@@ -4481,7 +4481,7 @@
         <v>194</v>
       </c>
       <c r="B194" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -4489,7 +4489,7 @@
         <v>195</v>
       </c>
       <c r="B195" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -4497,7 +4497,7 @@
         <v>196</v>
       </c>
       <c r="B196" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -4505,7 +4505,7 @@
         <v>197</v>
       </c>
       <c r="B197" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -4513,7 +4513,7 @@
         <v>198</v>
       </c>
       <c r="B198" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -4521,7 +4521,7 @@
         <v>199</v>
       </c>
       <c r="B199" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -4529,7 +4529,7 @@
         <v>200</v>
       </c>
       <c r="B200" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201">
@@ -4537,7 +4537,7 @@
         <v>201</v>
       </c>
       <c r="B201" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -4545,7 +4545,7 @@
         <v>202</v>
       </c>
       <c r="B202" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -4601,7 +4601,7 @@
         <v>209</v>
       </c>
       <c r="B209" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="210">
@@ -4609,7 +4609,7 @@
         <v>210</v>
       </c>
       <c r="B210" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="211">
@@ -4617,7 +4617,7 @@
         <v>211</v>
       </c>
       <c r="B211" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="212">
@@ -4625,7 +4625,7 @@
         <v>212</v>
       </c>
       <c r="B212" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="213">
@@ -4729,7 +4729,7 @@
         <v>225</v>
       </c>
       <c r="B225" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="226">
@@ -4737,7 +4737,7 @@
         <v>226</v>
       </c>
       <c r="B226" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="227">
@@ -4745,7 +4745,7 @@
         <v>227</v>
       </c>
       <c r="B227" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="228">
@@ -4753,7 +4753,7 @@
         <v>228</v>
       </c>
       <c r="B228" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="229">
@@ -4761,7 +4761,7 @@
         <v>229</v>
       </c>
       <c r="B229" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="230">
@@ -4769,7 +4769,7 @@
         <v>230</v>
       </c>
       <c r="B230" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="231">
@@ -4777,7 +4777,7 @@
         <v>231</v>
       </c>
       <c r="B231" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="232">
@@ -4801,7 +4801,7 @@
         <v>234</v>
       </c>
       <c r="B234" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235">
@@ -4809,7 +4809,7 @@
         <v>235</v>
       </c>
       <c r="B235" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236">
@@ -4817,7 +4817,7 @@
         <v>236</v>
       </c>
       <c r="B236" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -4825,7 +4825,7 @@
         <v>237</v>
       </c>
       <c r="B237" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238">
@@ -4833,7 +4833,7 @@
         <v>238</v>
       </c>
       <c r="B238" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239">
@@ -4841,7 +4841,7 @@
         <v>239</v>
       </c>
       <c r="B239" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240">
@@ -4849,7 +4849,7 @@
         <v>240</v>
       </c>
       <c r="B240" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241">
@@ -4857,7 +4857,7 @@
         <v>241</v>
       </c>
       <c r="B241" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -4865,7 +4865,7 @@
         <v>242</v>
       </c>
       <c r="B242" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -4873,7 +4873,7 @@
         <v>243</v>
       </c>
       <c r="B243" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244">
@@ -4881,7 +4881,7 @@
         <v>244</v>
       </c>
       <c r="B244" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245">
@@ -4889,7 +4889,7 @@
         <v>245</v>
       </c>
       <c r="B245" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246">
@@ -4929,7 +4929,7 @@
         <v>250</v>
       </c>
       <c r="B250" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="251">
@@ -4937,7 +4937,7 @@
         <v>251</v>
       </c>
       <c r="B251" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="252">
@@ -4945,7 +4945,7 @@
         <v>252</v>
       </c>
       <c r="B252" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="253">
@@ -4953,7 +4953,7 @@
         <v>253</v>
       </c>
       <c r="B253" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="254">
@@ -4961,7 +4961,7 @@
         <v>254</v>
       </c>
       <c r="B254" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="255">
@@ -5065,7 +5065,7 @@
         <v>267</v>
       </c>
       <c r="B267" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="268">
@@ -5073,7 +5073,7 @@
         <v>268</v>
       </c>
       <c r="B268" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="269">
@@ -5081,7 +5081,7 @@
         <v>269</v>
       </c>
       <c r="B269" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="270">
@@ -5089,7 +5089,7 @@
         <v>270</v>
       </c>
       <c r="B270" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="271">
@@ -5097,7 +5097,7 @@
         <v>271</v>
       </c>
       <c r="B271" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="272">
@@ -5105,7 +5105,7 @@
         <v>272</v>
       </c>
       <c r="B272" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="273">
@@ -5113,7 +5113,7 @@
         <v>273</v>
       </c>
       <c r="B273" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="274">
@@ -5121,7 +5121,7 @@
         <v>274</v>
       </c>
       <c r="B274" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="275">
@@ -5137,7 +5137,7 @@
         <v>276</v>
       </c>
       <c r="B276" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="277">
@@ -5145,7 +5145,7 @@
         <v>277</v>
       </c>
       <c r="B277" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278">
@@ -5153,7 +5153,7 @@
         <v>278</v>
       </c>
       <c r="B278" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279">
@@ -5161,7 +5161,7 @@
         <v>279</v>
       </c>
       <c r="B279" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280">
@@ -5169,7 +5169,7 @@
         <v>280</v>
       </c>
       <c r="B280" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281">
@@ -5177,7 +5177,7 @@
         <v>281</v>
       </c>
       <c r="B281" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282">
@@ -5185,7 +5185,7 @@
         <v>282</v>
       </c>
       <c r="B282" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283">
@@ -5193,7 +5193,7 @@
         <v>283</v>
       </c>
       <c r="B283" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284">
@@ -5201,7 +5201,7 @@
         <v>284</v>
       </c>
       <c r="B284" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285">
@@ -5209,7 +5209,7 @@
         <v>285</v>
       </c>
       <c r="B285" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286">
@@ -5217,7 +5217,7 @@
         <v>286</v>
       </c>
       <c r="B286" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287">
@@ -5225,7 +5225,7 @@
         <v>287</v>
       </c>
       <c r="B287" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288">
@@ -5233,7 +5233,7 @@
         <v>288</v>
       </c>
       <c r="B288" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="289">
@@ -5273,7 +5273,7 @@
         <v>293</v>
       </c>
       <c r="B293" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="294">
@@ -5281,7 +5281,7 @@
         <v>294</v>
       </c>
       <c r="B294" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="295">
@@ -5289,7 +5289,7 @@
         <v>295</v>
       </c>
       <c r="B295" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="296">
@@ -5297,7 +5297,7 @@
         <v>296</v>
       </c>
       <c r="B296" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="297">
@@ -5417,7 +5417,7 @@
         <v>311</v>
       </c>
       <c r="B311" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="312">
@@ -5425,7 +5425,7 @@
         <v>312</v>
       </c>
       <c r="B312" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="313">
@@ -5433,7 +5433,7 @@
         <v>313</v>
       </c>
       <c r="B313" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="314">
@@ -5441,7 +5441,7 @@
         <v>314</v>
       </c>
       <c r="B314" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="315">
@@ -5449,7 +5449,7 @@
         <v>315</v>
       </c>
       <c r="B315" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="316">
@@ -5457,7 +5457,7 @@
         <v>316</v>
       </c>
       <c r="B316" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="317">
@@ -5481,7 +5481,7 @@
         <v>319</v>
       </c>
       <c r="B319" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320">
@@ -5489,7 +5489,7 @@
         <v>320</v>
       </c>
       <c r="B320" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="321">
@@ -5497,7 +5497,7 @@
         <v>321</v>
       </c>
       <c r="B321" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322">
@@ -5505,7 +5505,7 @@
         <v>322</v>
       </c>
       <c r="B322" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323">
@@ -5513,7 +5513,7 @@
         <v>323</v>
       </c>
       <c r="B323" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324">
@@ -5521,7 +5521,7 @@
         <v>324</v>
       </c>
       <c r="B324" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="325">
@@ -5529,7 +5529,7 @@
         <v>325</v>
       </c>
       <c r="B325" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326">
@@ -5537,7 +5537,7 @@
         <v>326</v>
       </c>
       <c r="B326" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327">
@@ -5545,7 +5545,7 @@
         <v>327</v>
       </c>
       <c r="B327" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328">
@@ -5553,7 +5553,7 @@
         <v>328</v>
       </c>
       <c r="B328" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329">
@@ -5561,7 +5561,7 @@
         <v>329</v>
       </c>
       <c r="B329" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="330">
@@ -5569,7 +5569,7 @@
         <v>330</v>
       </c>
       <c r="B330" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331">
@@ -5577,7 +5577,7 @@
         <v>331</v>
       </c>
       <c r="B331" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="332">
@@ -5609,7 +5609,7 @@
         <v>335</v>
       </c>
       <c r="B335" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="336">
@@ -5617,7 +5617,7 @@
         <v>336</v>
       </c>
       <c r="B336" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="337">
@@ -5625,7 +5625,7 @@
         <v>337</v>
       </c>
       <c r="B337" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="338">
@@ -5633,7 +5633,7 @@
         <v>338</v>
       </c>
       <c r="B338" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="339">
@@ -5641,7 +5641,7 @@
         <v>339</v>
       </c>
       <c r="B339" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="340">
@@ -5761,7 +5761,7 @@
         <v>354</v>
       </c>
       <c r="B354" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="355">
@@ -5769,7 +5769,7 @@
         <v>355</v>
       </c>
       <c r="B355" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="356">
@@ -5777,7 +5777,7 @@
         <v>356</v>
       </c>
       <c r="B356" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="357">
@@ -5785,7 +5785,7 @@
         <v>357</v>
       </c>
       <c r="B357" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="358">
@@ -5793,7 +5793,7 @@
         <v>358</v>
       </c>
       <c r="B358" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="359">
@@ -5801,7 +5801,7 @@
         <v>359</v>
       </c>
       <c r="B359" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="360">
@@ -5809,7 +5809,7 @@
         <v>360</v>
       </c>
       <c r="B360" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="361">
@@ -5825,7 +5825,7 @@
         <v>362</v>
       </c>
       <c r="B362" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363">
@@ -5833,7 +5833,7 @@
         <v>363</v>
       </c>
       <c r="B363" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364">
@@ -5841,7 +5841,7 @@
         <v>364</v>
       </c>
       <c r="B364" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="365">
@@ -5849,7 +5849,7 @@
         <v>365</v>
       </c>
       <c r="B365" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="366">
@@ -5857,7 +5857,7 @@
         <v>366</v>
       </c>
       <c r="B366" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="367">
@@ -5865,7 +5865,7 @@
         <v>367</v>
       </c>
       <c r="B367" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="368">
@@ -5873,7 +5873,7 @@
         <v>368</v>
       </c>
       <c r="B368" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369">
@@ -5881,7 +5881,7 @@
         <v>369</v>
       </c>
       <c r="B369" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="370">
@@ -5889,7 +5889,7 @@
         <v>370</v>
       </c>
       <c r="B370" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="371">
@@ -5897,7 +5897,7 @@
         <v>371</v>
       </c>
       <c r="B371" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372">
@@ -5905,7 +5905,7 @@
         <v>372</v>
       </c>
       <c r="B372" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="373">
@@ -5913,7 +5913,7 @@
         <v>373</v>
       </c>
       <c r="B373" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="374">
@@ -5921,7 +5921,7 @@
         <v>374</v>
       </c>
       <c r="B374" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="375">
@@ -5945,7 +5945,7 @@
         <v>377</v>
       </c>
       <c r="B377" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="378">
@@ -5953,7 +5953,7 @@
         <v>378</v>
       </c>
       <c r="B378" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="379">
@@ -5961,7 +5961,7 @@
         <v>379</v>
       </c>
       <c r="B379" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="380">
@@ -5969,7 +5969,7 @@
         <v>380</v>
       </c>
       <c r="B380" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="381">
@@ -5977,7 +5977,7 @@
         <v>381</v>
       </c>
       <c r="B381" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="382">
@@ -5985,7 +5985,7 @@
         <v>382</v>
       </c>
       <c r="B382" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="383">
@@ -6097,7 +6097,7 @@
         <v>396</v>
       </c>
       <c r="B396" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="397">
@@ -6105,7 +6105,7 @@
         <v>397</v>
       </c>
       <c r="B397" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="398">
@@ -6113,7 +6113,7 @@
         <v>398</v>
       </c>
       <c r="B398" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="399">
@@ -6121,7 +6121,7 @@
         <v>399</v>
       </c>
       <c r="B399" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="400">
@@ -6129,7 +6129,7 @@
         <v>400</v>
       </c>
       <c r="B400" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="401">
@@ -6137,7 +6137,7 @@
         <v>401</v>
       </c>
       <c r="B401" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="402">
@@ -6145,7 +6145,7 @@
         <v>402</v>
       </c>
       <c r="B402" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="403">
@@ -6161,7 +6161,7 @@
         <v>404</v>
       </c>
       <c r="B404" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="405">
@@ -6169,7 +6169,7 @@
         <v>405</v>
       </c>
       <c r="B405" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="406">
@@ -6177,7 +6177,7 @@
         <v>406</v>
       </c>
       <c r="B406" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="407">
@@ -6185,7 +6185,7 @@
         <v>407</v>
       </c>
       <c r="B407" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="408">
@@ -6193,7 +6193,7 @@
         <v>408</v>
       </c>
       <c r="B408" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="409">
@@ -6201,7 +6201,7 @@
         <v>409</v>
       </c>
       <c r="B409" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410">
@@ -6209,7 +6209,7 @@
         <v>410</v>
       </c>
       <c r="B410" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="411">
@@ -6217,7 +6217,7 @@
         <v>411</v>
       </c>
       <c r="B411" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412">
@@ -6225,7 +6225,7 @@
         <v>412</v>
       </c>
       <c r="B412" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="413">
@@ -6233,7 +6233,7 @@
         <v>413</v>
       </c>
       <c r="B413" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="414">
@@ -6241,7 +6241,7 @@
         <v>414</v>
       </c>
       <c r="B414" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="415">
@@ -6249,7 +6249,7 @@
         <v>415</v>
       </c>
       <c r="B415" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="416">
@@ -6257,7 +6257,7 @@
         <v>416</v>
       </c>
       <c r="B416" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="417">
@@ -6265,7 +6265,7 @@
         <v>417</v>
       </c>
       <c r="B417" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418">
@@ -6289,7 +6289,7 @@
         <v>420</v>
       </c>
       <c r="B420" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="421">
@@ -6297,7 +6297,7 @@
         <v>421</v>
       </c>
       <c r="B421" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="422">
@@ -6305,7 +6305,7 @@
         <v>422</v>
       </c>
       <c r="B422" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="423">
@@ -6313,7 +6313,7 @@
         <v>423</v>
       </c>
       <c r="B423" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="424">
@@ -6321,7 +6321,7 @@
         <v>424</v>
       </c>
       <c r="B424" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="425">
@@ -6329,7 +6329,7 @@
         <v>425</v>
       </c>
       <c r="B425" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="426">
@@ -6441,7 +6441,7 @@
         <v>439</v>
       </c>
       <c r="B439" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="440">
@@ -6449,7 +6449,7 @@
         <v>440</v>
       </c>
       <c r="B440" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="441">
@@ -6457,7 +6457,7 @@
         <v>441</v>
       </c>
       <c r="B441" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="442">
@@ -6465,7 +6465,7 @@
         <v>442</v>
       </c>
       <c r="B442" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="443">
@@ -6473,7 +6473,7 @@
         <v>443</v>
       </c>
       <c r="B443" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="444">
@@ -6481,7 +6481,7 @@
         <v>444</v>
       </c>
       <c r="B444" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="445">
@@ -6505,7 +6505,7 @@
         <v>447</v>
       </c>
       <c r="B447" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="448">
@@ -6513,7 +6513,7 @@
         <v>448</v>
       </c>
       <c r="B448" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="449">
@@ -6521,7 +6521,7 @@
         <v>449</v>
       </c>
       <c r="B449" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="450">
@@ -6529,7 +6529,7 @@
         <v>450</v>
       </c>
       <c r="B450" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="451">
@@ -6537,7 +6537,7 @@
         <v>451</v>
       </c>
       <c r="B451" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="452">
@@ -6545,7 +6545,7 @@
         <v>452</v>
       </c>
       <c r="B452" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="453">
@@ -6553,7 +6553,7 @@
         <v>453</v>
       </c>
       <c r="B453" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="454">
@@ -6561,7 +6561,7 @@
         <v>454</v>
       </c>
       <c r="B454" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="455">
@@ -6569,7 +6569,7 @@
         <v>455</v>
       </c>
       <c r="B455" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="456">
@@ -6577,7 +6577,7 @@
         <v>456</v>
       </c>
       <c r="B456" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="457">
@@ -6585,7 +6585,7 @@
         <v>457</v>
       </c>
       <c r="B457" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="458">
@@ -6593,7 +6593,7 @@
         <v>458</v>
       </c>
       <c r="B458" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="459">
@@ -6601,7 +6601,7 @@
         <v>459</v>
       </c>
       <c r="B459" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="460">
@@ -6609,7 +6609,7 @@
         <v>460</v>
       </c>
       <c r="B460" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="461">
@@ -6625,7 +6625,7 @@
         <v>462</v>
       </c>
       <c r="B462" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="463">
@@ -6633,7 +6633,7 @@
         <v>463</v>
       </c>
       <c r="B463" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="464">
@@ -6641,7 +6641,7 @@
         <v>464</v>
       </c>
       <c r="B464" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="465">
@@ -6649,7 +6649,7 @@
         <v>465</v>
       </c>
       <c r="B465" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="466">
@@ -6657,7 +6657,7 @@
         <v>466</v>
       </c>
       <c r="B466" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="467">
@@ -6665,7 +6665,7 @@
         <v>467</v>
       </c>
       <c r="B467" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="468">
@@ -6673,7 +6673,7 @@
         <v>468</v>
       </c>
       <c r="B468" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="469">
@@ -6785,7 +6785,7 @@
         <v>482</v>
       </c>
       <c r="B482" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="483">
@@ -6793,7 +6793,7 @@
         <v>483</v>
       </c>
       <c r="B483" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="484">
@@ -6801,7 +6801,7 @@
         <v>484</v>
       </c>
       <c r="B484" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="485">
@@ -6809,7 +6809,7 @@
         <v>485</v>
       </c>
       <c r="B485" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="486">
@@ -6817,7 +6817,7 @@
         <v>486</v>
       </c>
       <c r="B486" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="487">
@@ -6825,7 +6825,7 @@
         <v>487</v>
       </c>
       <c r="B487" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="488">
@@ -6849,7 +6849,7 @@
         <v>490</v>
       </c>
       <c r="B490" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="491">
@@ -6857,7 +6857,7 @@
         <v>491</v>
       </c>
       <c r="B491" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="492">
@@ -6865,7 +6865,7 @@
         <v>492</v>
       </c>
       <c r="B492" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="493">
@@ -6873,7 +6873,7 @@
         <v>493</v>
       </c>
       <c r="B493" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="494">
@@ -6881,7 +6881,7 @@
         <v>494</v>
       </c>
       <c r="B494" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="495">
@@ -6889,7 +6889,7 @@
         <v>495</v>
       </c>
       <c r="B495" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="496">
@@ -6897,7 +6897,7 @@
         <v>496</v>
       </c>
       <c r="B496" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="497">
@@ -6905,7 +6905,7 @@
         <v>497</v>
       </c>
       <c r="B497" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="498">
@@ -6913,7 +6913,7 @@
         <v>498</v>
       </c>
       <c r="B498" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="499">
@@ -6921,7 +6921,7 @@
         <v>499</v>
       </c>
       <c r="B499" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="500">
@@ -6929,7 +6929,7 @@
         <v>500</v>
       </c>
       <c r="B500" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="501">
@@ -6937,7 +6937,7 @@
         <v>501</v>
       </c>
       <c r="B501" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="502">
@@ -6945,7 +6945,7 @@
         <v>502</v>
       </c>
       <c r="B502" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="503">
@@ -6961,7 +6961,7 @@
         <v>504</v>
       </c>
       <c r="B504" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="505">
@@ -6969,7 +6969,7 @@
         <v>505</v>
       </c>
       <c r="B505" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="506">
@@ -6977,7 +6977,7 @@
         <v>506</v>
       </c>
       <c r="B506" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="507">
@@ -6985,7 +6985,7 @@
         <v>507</v>
       </c>
       <c r="B507" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="508">
@@ -6993,7 +6993,7 @@
         <v>508</v>
       </c>
       <c r="B508" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="509">
@@ -7001,7 +7001,7 @@
         <v>509</v>
       </c>
       <c r="B509" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="510">
@@ -7009,7 +7009,7 @@
         <v>510</v>
       </c>
       <c r="B510" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="511">
@@ -7129,7 +7129,7 @@
         <v>525</v>
       </c>
       <c r="B525" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="526">
@@ -7137,7 +7137,7 @@
         <v>526</v>
       </c>
       <c r="B526" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="527">
@@ -7145,7 +7145,7 @@
         <v>527</v>
       </c>
       <c r="B527" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="528">
@@ -7153,7 +7153,7 @@
         <v>528</v>
       </c>
       <c r="B528" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="529">
@@ -7161,7 +7161,7 @@
         <v>529</v>
       </c>
       <c r="B529" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="530">
@@ -7193,7 +7193,7 @@
         <v>533</v>
       </c>
       <c r="B533" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="534">
@@ -7201,7 +7201,7 @@
         <v>534</v>
       </c>
       <c r="B534" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="535">
@@ -7209,7 +7209,7 @@
         <v>535</v>
       </c>
       <c r="B535" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="536">
@@ -7217,7 +7217,7 @@
         <v>536</v>
       </c>
       <c r="B536" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="537">
@@ -7225,7 +7225,7 @@
         <v>537</v>
       </c>
       <c r="B537" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="538">
@@ -7233,7 +7233,7 @@
         <v>538</v>
       </c>
       <c r="B538" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="539">
@@ -7241,7 +7241,7 @@
         <v>539</v>
       </c>
       <c r="B539" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="540">
@@ -7249,7 +7249,7 @@
         <v>540</v>
       </c>
       <c r="B540" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="541">
@@ -7257,7 +7257,7 @@
         <v>541</v>
       </c>
       <c r="B541" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="542">
@@ -7265,7 +7265,7 @@
         <v>542</v>
       </c>
       <c r="B542" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="543">
@@ -7273,7 +7273,7 @@
         <v>543</v>
       </c>
       <c r="B543" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="544">
@@ -7281,7 +7281,7 @@
         <v>544</v>
       </c>
       <c r="B544" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="545">
@@ -7289,7 +7289,7 @@
         <v>545</v>
       </c>
       <c r="B545" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="546">
@@ -7313,7 +7313,7 @@
         <v>548</v>
       </c>
       <c r="B548" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="549">
@@ -7321,7 +7321,7 @@
         <v>549</v>
       </c>
       <c r="B549" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="550">
@@ -7329,7 +7329,7 @@
         <v>550</v>
       </c>
       <c r="B550" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="551">
@@ -7337,7 +7337,7 @@
         <v>551</v>
       </c>
       <c r="B551" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="552">
@@ -7345,7 +7345,7 @@
         <v>552</v>
       </c>
       <c r="B552" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="553">
@@ -7353,7 +7353,7 @@
         <v>553</v>
       </c>
       <c r="B553" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="554">
@@ -7473,7 +7473,7 @@
         <v>568</v>
       </c>
       <c r="B568" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="569">
@@ -7481,7 +7481,7 @@
         <v>569</v>
       </c>
       <c r="B569" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="570">
@@ -7489,7 +7489,7 @@
         <v>570</v>
       </c>
       <c r="B570" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="571">
@@ -7497,7 +7497,7 @@
         <v>571</v>
       </c>
       <c r="B571" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="572">
@@ -7537,7 +7537,7 @@
         <v>576</v>
       </c>
       <c r="B576" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="577">
@@ -7545,7 +7545,7 @@
         <v>577</v>
       </c>
       <c r="B577" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="578">
@@ -7553,7 +7553,7 @@
         <v>578</v>
       </c>
       <c r="B578" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="579">
@@ -7561,7 +7561,7 @@
         <v>579</v>
       </c>
       <c r="B579" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="580">
@@ -7569,7 +7569,7 @@
         <v>580</v>
       </c>
       <c r="B580" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="581">
@@ -7577,7 +7577,7 @@
         <v>581</v>
       </c>
       <c r="B581" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="582">
@@ -7585,7 +7585,7 @@
         <v>582</v>
       </c>
       <c r="B582" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="583">
@@ -7593,7 +7593,7 @@
         <v>583</v>
       </c>
       <c r="B583" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="584">
@@ -7601,7 +7601,7 @@
         <v>584</v>
       </c>
       <c r="B584" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="585">
@@ -7609,7 +7609,7 @@
         <v>585</v>
       </c>
       <c r="B585" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="586">
@@ -7617,7 +7617,7 @@
         <v>586</v>
       </c>
       <c r="B586" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="587">
@@ -7625,7 +7625,7 @@
         <v>587</v>
       </c>
       <c r="B587" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="588">
@@ -7633,7 +7633,7 @@
         <v>588</v>
       </c>
       <c r="B588" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="589">
@@ -7649,7 +7649,7 @@
         <v>590</v>
       </c>
       <c r="B590" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="591">
@@ -7657,7 +7657,7 @@
         <v>591</v>
       </c>
       <c r="B591" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="592">
@@ -7665,7 +7665,7 @@
         <v>592</v>
       </c>
       <c r="B592" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="593">
@@ -7673,7 +7673,7 @@
         <v>593</v>
       </c>
       <c r="B593" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="594">
@@ -7681,7 +7681,7 @@
         <v>594</v>
       </c>
       <c r="B594" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="595">
@@ -7689,7 +7689,7 @@
         <v>595</v>
       </c>
       <c r="B595" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="596">
@@ -7697,7 +7697,7 @@
         <v>596</v>
       </c>
       <c r="B596" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="597">
@@ -7705,7 +7705,7 @@
         <v>597</v>
       </c>
       <c r="B597" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="598">
@@ -7809,7 +7809,7 @@
         <v>610</v>
       </c>
       <c r="B610" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="611">
@@ -7817,7 +7817,7 @@
         <v>611</v>
       </c>
       <c r="B611" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="612">
@@ -7825,7 +7825,7 @@
         <v>612</v>
       </c>
       <c r="B612" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="613">
@@ -7833,7 +7833,7 @@
         <v>613</v>
       </c>
       <c r="B613" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="614">
@@ -7841,7 +7841,7 @@
         <v>614</v>
       </c>
       <c r="B614" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="615">
@@ -7881,7 +7881,7 @@
         <v>619</v>
       </c>
       <c r="B619" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="620">
@@ -7889,7 +7889,7 @@
         <v>620</v>
       </c>
       <c r="B620" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="621">
@@ -7897,7 +7897,7 @@
         <v>621</v>
       </c>
       <c r="B621" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="622">
@@ -7905,7 +7905,7 @@
         <v>622</v>
       </c>
       <c r="B622" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="623">
@@ -7913,7 +7913,7 @@
         <v>623</v>
       </c>
       <c r="B623" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="624">
@@ -7921,7 +7921,7 @@
         <v>624</v>
       </c>
       <c r="B624" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="625">
@@ -7929,7 +7929,7 @@
         <v>625</v>
       </c>
       <c r="B625" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="626">
@@ -7937,7 +7937,7 @@
         <v>626</v>
       </c>
       <c r="B626" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="627">
@@ -7945,7 +7945,7 @@
         <v>627</v>
       </c>
       <c r="B627" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="628">
@@ -7953,7 +7953,7 @@
         <v>628</v>
       </c>
       <c r="B628" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="629">
@@ -7961,7 +7961,7 @@
         <v>629</v>
       </c>
       <c r="B629" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="630">
@@ -7969,7 +7969,7 @@
         <v>630</v>
       </c>
       <c r="B630" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="631">
@@ -7993,7 +7993,7 @@
         <v>633</v>
       </c>
       <c r="B633" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="634">
@@ -8001,7 +8001,7 @@
         <v>634</v>
       </c>
       <c r="B634" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="635">
@@ -8009,7 +8009,7 @@
         <v>635</v>
       </c>
       <c r="B635" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="636">
@@ -8017,7 +8017,7 @@
         <v>636</v>
       </c>
       <c r="B636" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="637">
@@ -8025,7 +8025,7 @@
         <v>637</v>
       </c>
       <c r="B637" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="638">
@@ -8033,7 +8033,7 @@
         <v>638</v>
       </c>
       <c r="B638" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="639">
@@ -8041,7 +8041,7 @@
         <v>639</v>
       </c>
       <c r="B639" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="640">
@@ -8145,7 +8145,7 @@
         <v>652</v>
       </c>
       <c r="B652" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="653">
@@ -8153,7 +8153,7 @@
         <v>653</v>
       </c>
       <c r="B653" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="654">
@@ -8161,7 +8161,7 @@
         <v>654</v>
       </c>
       <c r="B654" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="655">
@@ -8169,7 +8169,7 @@
         <v>655</v>
       </c>
       <c r="B655" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="656">
@@ -8225,7 +8225,7 @@
         <v>662</v>
       </c>
       <c r="B662" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="663">
@@ -8233,7 +8233,7 @@
         <v>663</v>
       </c>
       <c r="B663" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="664">
@@ -8241,7 +8241,7 @@
         <v>664</v>
       </c>
       <c r="B664" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="665">
@@ -8249,7 +8249,7 @@
         <v>665</v>
       </c>
       <c r="B665" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="666">
@@ -8257,7 +8257,7 @@
         <v>666</v>
       </c>
       <c r="B666" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="667">
@@ -8265,7 +8265,7 @@
         <v>667</v>
       </c>
       <c r="B667" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="668">
@@ -8273,7 +8273,7 @@
         <v>668</v>
       </c>
       <c r="B668" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="669">
@@ -8281,7 +8281,7 @@
         <v>669</v>
       </c>
       <c r="B669" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="670">
@@ -8289,7 +8289,7 @@
         <v>670</v>
       </c>
       <c r="B670" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="671">
@@ -8297,7 +8297,7 @@
         <v>671</v>
       </c>
       <c r="B671" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="672">
@@ -8305,7 +8305,7 @@
         <v>672</v>
       </c>
       <c r="B672" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="673">
@@ -8313,7 +8313,7 @@
         <v>673</v>
       </c>
       <c r="B673" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="674">
@@ -8345,7 +8345,7 @@
         <v>677</v>
       </c>
       <c r="B677" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="678">
@@ -8353,7 +8353,7 @@
         <v>678</v>
       </c>
       <c r="B678" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="679">
@@ -8361,7 +8361,7 @@
         <v>679</v>
       </c>
       <c r="B679" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="680">
@@ -8369,7 +8369,7 @@
         <v>680</v>
       </c>
       <c r="B680" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="681">
@@ -8377,7 +8377,7 @@
         <v>681</v>
       </c>
       <c r="B681" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="682">
@@ -8385,7 +8385,7 @@
         <v>682</v>
       </c>
       <c r="B682" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="683">
@@ -8393,7 +8393,7 @@
         <v>683</v>
       </c>
       <c r="B683" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="684">
@@ -8489,7 +8489,7 @@
         <v>695</v>
       </c>
       <c r="B695" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="696">
@@ -8497,7 +8497,7 @@
         <v>696</v>
       </c>
       <c r="B696" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="697">
@@ -8505,7 +8505,7 @@
         <v>697</v>
       </c>
       <c r="B697" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="698">
@@ -8577,7 +8577,7 @@
         <v>706</v>
       </c>
       <c r="B706" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="707">
@@ -8585,7 +8585,7 @@
         <v>707</v>
       </c>
       <c r="B707" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="708">
@@ -8593,7 +8593,7 @@
         <v>708</v>
       </c>
       <c r="B708" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="709">
@@ -8601,7 +8601,7 @@
         <v>709</v>
       </c>
       <c r="B709" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="710">
@@ -8609,7 +8609,7 @@
         <v>710</v>
       </c>
       <c r="B710" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="711">
@@ -8617,7 +8617,7 @@
         <v>711</v>
       </c>
       <c r="B711" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="712">
@@ -8625,7 +8625,7 @@
         <v>712</v>
       </c>
       <c r="B712" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="713">
@@ -8633,7 +8633,7 @@
         <v>713</v>
       </c>
       <c r="B713" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="714">
@@ -8641,7 +8641,7 @@
         <v>714</v>
       </c>
       <c r="B714" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="715">
@@ -8649,7 +8649,7 @@
         <v>715</v>
       </c>
       <c r="B715" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="716">
@@ -8689,7 +8689,7 @@
         <v>720</v>
       </c>
       <c r="B720" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="721">
@@ -8697,7 +8697,7 @@
         <v>721</v>
       </c>
       <c r="B721" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="722">
@@ -8705,7 +8705,7 @@
         <v>722</v>
       </c>
       <c r="B722" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="723">
@@ -8713,7 +8713,7 @@
         <v>723</v>
       </c>
       <c r="B723" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="724">
@@ -8721,7 +8721,7 @@
         <v>724</v>
       </c>
       <c r="B724" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="725">
@@ -8729,7 +8729,7 @@
         <v>725</v>
       </c>
       <c r="B725" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="726">
@@ -8737,7 +8737,7 @@
         <v>726</v>
       </c>
       <c r="B726" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="727">
@@ -8825,7 +8825,7 @@
         <v>737</v>
       </c>
       <c r="B737" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="738">
@@ -8833,7 +8833,7 @@
         <v>738</v>
       </c>
       <c r="B738" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="739">
@@ -8841,7 +8841,7 @@
         <v>739</v>
       </c>
       <c r="B739" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="740">
@@ -8921,7 +8921,7 @@
         <v>749</v>
       </c>
       <c r="B749" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="750">
@@ -8929,7 +8929,7 @@
         <v>750</v>
       </c>
       <c r="B750" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="751">
@@ -8937,7 +8937,7 @@
         <v>751</v>
       </c>
       <c r="B751" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="752">
@@ -8945,7 +8945,7 @@
         <v>752</v>
       </c>
       <c r="B752" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="753">
@@ -8953,7 +8953,7 @@
         <v>753</v>
       </c>
       <c r="B753" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="754">
@@ -8961,7 +8961,7 @@
         <v>754</v>
       </c>
       <c r="B754" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="755">
@@ -8969,7 +8969,7 @@
         <v>755</v>
       </c>
       <c r="B755" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="756">
@@ -8977,7 +8977,7 @@
         <v>756</v>
       </c>
       <c r="B756" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="757">
@@ -8985,7 +8985,7 @@
         <v>757</v>
       </c>
       <c r="B757" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="758">
@@ -9041,7 +9041,7 @@
         <v>764</v>
       </c>
       <c r="B764" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="765">
@@ -9049,7 +9049,7 @@
         <v>765</v>
       </c>
       <c r="B765" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="766">
@@ -9057,7 +9057,7 @@
         <v>766</v>
       </c>
       <c r="B766" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="767">
@@ -9065,7 +9065,7 @@
         <v>767</v>
       </c>
       <c r="B767" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="768">
@@ -9073,7 +9073,7 @@
         <v>768</v>
       </c>
       <c r="B768" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="769">
@@ -9081,7 +9081,7 @@
         <v>769</v>
       </c>
       <c r="B769" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="770">
@@ -9089,7 +9089,7 @@
         <v>770</v>
       </c>
       <c r="B770" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="771">
@@ -9161,7 +9161,7 @@
         <v>779</v>
       </c>
       <c r="B779" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="780">
@@ -9169,7 +9169,7 @@
         <v>780</v>
       </c>
       <c r="B780" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="781">
@@ -9273,7 +9273,7 @@
         <v>793</v>
       </c>
       <c r="B793" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="794">
@@ -9281,7 +9281,7 @@
         <v>794</v>
       </c>
       <c r="B794" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="795">
@@ -9289,7 +9289,7 @@
         <v>795</v>
       </c>
       <c r="B795" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="796">
@@ -9297,7 +9297,7 @@
         <v>796</v>
       </c>
       <c r="B796" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="797">
@@ -9305,7 +9305,7 @@
         <v>797</v>
       </c>
       <c r="B797" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="798">
@@ -9313,7 +9313,7 @@
         <v>798</v>
       </c>
       <c r="B798" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="799">
@@ -9321,7 +9321,7 @@
         <v>799</v>
       </c>
       <c r="B799" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="800">
@@ -9385,7 +9385,7 @@
         <v>807</v>
       </c>
       <c r="B807" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="808">
@@ -9393,7 +9393,7 @@
         <v>808</v>
       </c>
       <c r="B808" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="809">
@@ -9401,7 +9401,7 @@
         <v>809</v>
       </c>
       <c r="B809" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="810">
@@ -9409,7 +9409,7 @@
         <v>810</v>
       </c>
       <c r="B810" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="811">
@@ -9417,7 +9417,7 @@
         <v>811</v>
       </c>
       <c r="B811" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="812">
@@ -9425,7 +9425,7 @@
         <v>812</v>
       </c>
       <c r="B812" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="813">
@@ -9433,7 +9433,7 @@
         <v>813</v>
       </c>
       <c r="B813" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="814">
@@ -9497,7 +9497,7 @@
         <v>821</v>
       </c>
       <c r="B821" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="822">
@@ -9625,7 +9625,7 @@
         <v>837</v>
       </c>
       <c r="B837" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="838">
@@ -9633,7 +9633,7 @@
         <v>838</v>
       </c>
       <c r="B838" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="839">
@@ -9641,7 +9641,7 @@
         <v>839</v>
       </c>
       <c r="B839" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="840">
@@ -9649,7 +9649,7 @@
         <v>840</v>
       </c>
       <c r="B840" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="841">
@@ -9657,7 +9657,7 @@
         <v>841</v>
       </c>
       <c r="B841" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="842">
@@ -9753,7 +9753,7 @@
         <v>853</v>
       </c>
       <c r="B853" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="854">
@@ -9761,7 +9761,7 @@
         <v>854</v>
       </c>
       <c r="B854" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="855">
@@ -9769,7 +9769,7 @@
         <v>855</v>
       </c>
       <c r="B855" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="856">
@@ -9777,7 +9777,7 @@
         <v>856</v>
       </c>
       <c r="B856" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="857">
@@ -9785,7 +9785,7 @@
         <v>857</v>
       </c>
       <c r="B857" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="858">
@@ -9793,7 +9793,7 @@
         <v>858</v>
       </c>
       <c r="B858" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="859">

</xml_diff>